<commit_message>
Added oscillator strengths for each line
</commit_message>
<xml_diff>
--- a/data/bright_lines.xlsx
+++ b/data/bright_lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojoa\GitHub\io_brightness\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03ED17E-ED23-41AC-A32C-2F710DC54774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FDF48C-AE8A-428F-A139-DD5F666D38BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{DFAE8F92-55DC-47F1-9DEE-F1EEFF5E956D}"/>
+    <workbookView xWindow="16230" yWindow="3700" windowWidth="7500" windowHeight="6000" xr2:uid="{DFAE8F92-55DC-47F1-9DEE-F1EEFF5E956D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
   <si>
     <t>Wavelength</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Lower State</t>
-  </si>
-  <si>
-    <t>Upper State</t>
-  </si>
-  <si>
     <t>O I</t>
   </si>
   <si>
@@ -156,12 +150,6 @@
     <t>Optically thick, self absorbed</t>
   </si>
   <si>
-    <t>1355.598</t>
-  </si>
-  <si>
-    <t>1358.512</t>
-  </si>
-  <si>
     <t>1379.528</t>
   </si>
   <si>
@@ -186,17 +174,17 @@
     <t>Solar Si IV at 1402.6 useful for albedo</t>
   </si>
   <si>
-    <t>S IV</t>
-  </si>
-  <si>
-    <t>1.64e+04 </t>
+    <t>Oscillator Strength</t>
+  </si>
+  <si>
+    <t>Amplitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +229,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,6 +306,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,19 +621,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118718B6-5B67-4462-BC0A-B1278D1F5110}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="69.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,599 +646,670 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>1152.1510000000001</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="17">
+        <v>2640000000</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="6">
+        <v>528000000</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6">
-        <v>528000000</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="8">
         <v>1188.7739999999999</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="17">
+        <v>1400000000</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="11">
         <v>233000000</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8">
         <v>1190.2059999999999</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="17">
+        <v>122000000</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="11">
         <v>40500000</v>
       </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="8">
         <v>1194.0609999999999</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="17">
+        <v>269000000</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="G5" s="11">
+        <v>53800000</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="17">
+        <v>463000000</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11">
-        <v>53800000</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="G6" s="11">
+        <v>66200000</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="D7" s="17">
+        <v>236000000</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="11">
-        <v>66200000</v>
-      </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="G7" s="13">
         <v>59100000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="8">
         <v>1204.335</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="13">
+        <v>16</v>
+      </c>
+      <c r="D8" s="17">
+        <v>347000000</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="13">
         <v>57900000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="9">
         <v>1250.578</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="17">
+        <v>347000000</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="13">
+        <v>51300000</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="13">
-        <v>51300000</v>
-      </c>
-      <c r="F9" s="10" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="17">
+        <v>7980000</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2660000</v>
+      </c>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="17">
+        <v>205000000</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="13">
-        <v>2660000</v>
-      </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="13">
+      <c r="G11" s="13">
         <v>51200000</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H11" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="9">
         <v>1259.518</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="13">
+        <v>16</v>
+      </c>
+      <c r="D12" s="17">
+        <v>306000000</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="13">
         <v>51000000</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="H12" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="17">
+        <v>178000000</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="13">
+        <v>25400000</v>
+      </c>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+      <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="17">
+        <v>1730000000</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
+        <v>346000000</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="13">
-        <v>25400000</v>
-      </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+      <c r="B15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="17">
+        <v>1020000000</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="13">
+        <v>341000000</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="6">
-        <v>346000000</v>
-      </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+    </row>
+    <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="13">
-        <v>341000000</v>
-      </c>
-      <c r="F15" s="10" t="s">
+      <c r="B16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="17">
+        <v>600000000</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+      <c r="G16" s="13">
+        <v>120000000</v>
+      </c>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="4" t="s">
+      <c r="B17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="17">
+        <v>609000000</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="13">
+        <v>203000000</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="13">
-        <v>120000000</v>
-      </c>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="17">
+        <v>588000000</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="13">
+        <v>196000000</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="13">
+      <c r="B19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="17">
         <v>203000000</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="13">
-        <v>196000000</v>
-      </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="13">
+      <c r="E19" s="10"/>
+      <c r="F19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="13">
         <v>67600000</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H19" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="9">
         <v>1316.5419999999999</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="13">
+      <c r="D20" s="17">
+        <v>552000000</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="13">
         <v>78900000</v>
       </c>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="13">
+      <c r="D21" s="17">
+        <v>105000000</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="13">
         <v>21000000</v>
       </c>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="9">
         <v>1323.5150000000001</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="13">
+        <v>18</v>
+      </c>
+      <c r="D22" s="17">
+        <v>302000000</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="13">
         <v>60400000</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H22" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A23" s="9">
         <v>1323.5219999999999</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="13">
+        <v>18</v>
+      </c>
+      <c r="D23" s="17">
+        <v>102000000</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="13">
         <v>34000000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="17">
+        <v>1680000000</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="13">
+        <v>419000000</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="13">
-        <v>419000000</v>
-      </c>
-      <c r="F24" s="10" t="s">
+      <c r="D25" s="17">
+        <v>44000000</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="13">
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="B26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="17">
+        <v>1630000</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="13">
+        <v>542000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="B27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="17">
+        <v>1250000</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="9">
+        <v>1388.4349999999999</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="17">
+        <v>2770000</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="13">
+        <v>554000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="9">
+        <v>1389.693</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="13">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+      <c r="D29" s="17">
+        <v>1400000</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="13">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+      <c r="G29" s="13">
+        <v>230000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="9">
+        <v>1392.588</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="17">
+        <v>1550000</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="13">
+        <v>516000</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="9">
+        <v>1396.1120000000001</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="17">
+        <v>2880000</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="13">
+        <v>575000</v>
+      </c>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="9">
+        <v>1401.5139999999999</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="17">
+        <v>4880</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="9">
+        <v>1409.337</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="17">
+        <v>130000000</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="13">
+        <v>43500000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="16">
+        <v>1425.2190000000001</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="17">
+        <v>31500000</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="13">
-        <v>11000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="13">
-        <v>542000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="13">
-        <v>1250000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="9">
-        <v>1388.4349999999999</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="13">
-        <v>554000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="9">
-        <v>1389.693</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="13">
-        <v>230000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="9">
-        <v>1392.588</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="13">
-        <v>516000</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="9">
-        <v>1396.1120000000001</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="13">
-        <v>575000</v>
-      </c>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="9">
-        <v>1401.5139999999999</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="9">
-        <v>1409.337</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="13">
-        <v>43500000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="9">
-        <v>1416.8869999999999</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="16">
-        <v>1425.2190000000001</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="13">
+      <c r="G34" s="13">
         <v>10500000</v>
       </c>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
-      <c r="B38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
-      <c r="B39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="9"/>
+      <c r="B35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="9"/>
+      <c r="B36" s="4"/>
+      <c r="F36" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added amplitudes with ratio calculation
</commit_message>
<xml_diff>
--- a/data/bright_lines.xlsx
+++ b/data/bright_lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojoa\GitHub\io_brightness\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FDF48C-AE8A-428F-A139-DD5F666D38BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0853BF40-CD6A-4988-B1EB-218556258607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16230" yWindow="3700" windowWidth="7500" windowHeight="6000" xr2:uid="{DFAE8F92-55DC-47F1-9DEE-F1EEFF5E956D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
   <si>
     <t>Wavelength</t>
   </si>
@@ -178,13 +178,19 @@
   </si>
   <si>
     <t>Amplitude</t>
+  </si>
+  <si>
+    <t>1425.030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S IV contributes negligibly </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,19 +228,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -256,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -303,10 +296,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,16 +610,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118718B6-5B67-4462-BC0A-B1278D1F5110}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="69.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -661,7 +652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1152.1510000000001</v>
       </c>
@@ -669,10 +660,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="17">
+      <c r="D2" s="6">
         <v>2640000000</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="6">
+        <f>3.28E-24*D2</f>
+        <v>8.6592E-15</v>
+      </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
@@ -683,7 +677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>1188.7739999999999</v>
       </c>
@@ -691,10 +685,13 @@
         <v>9</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="17">
+      <c r="D3" s="6">
         <v>1400000000</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E34" si="0">3.28E-24*D3</f>
+        <v>4.5919999999999997E-15</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
@@ -703,7 +700,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>1190.2059999999999</v>
       </c>
@@ -711,10 +708,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="17">
+      <c r="D4" s="6">
         <v>122000000</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0015999999999998E-16</v>
+      </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
@@ -723,7 +723,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>1194.0609999999999</v>
       </c>
@@ -731,10 +731,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="17">
+      <c r="D5" s="6">
         <v>269000000</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>8.8232000000000001E-16</v>
+      </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
@@ -743,7 +746,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -751,10 +754,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="17">
+      <c r="D6" s="6">
         <v>463000000</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>1.51864E-15</v>
+      </c>
       <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
@@ -763,15 +769,19 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="6">
         <v>236000000</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>7.7407999999999995E-16</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>13</v>
@@ -780,15 +790,19 @@
         <v>59100000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>1204.335</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="6">
         <v>347000000</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1381599999999999E-15</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>13</v>
@@ -797,15 +811,19 @@
         <v>57900000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>1250.578</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="6">
         <v>347000000</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1381599999999999E-15</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>19</v>
@@ -817,15 +835,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="6">
         <v>7980000</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6174399999999998E-17</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>20</v>
@@ -835,15 +857,19 @@
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="6">
         <v>205000000</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>6.7239999999999994E-16</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>20</v>
@@ -855,15 +881,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>1259.518</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="6">
         <v>306000000</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>1.00368E-15</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>7</v>
@@ -875,15 +905,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="6">
         <v>178000000</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>5.8383999999999994E-16</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>7</v>
@@ -893,7 +927,7 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>26</v>
       </c>
@@ -901,10 +935,13 @@
         <v>18</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="17">
+      <c r="D14" s="6">
         <v>1730000000</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>5.6744000000000001E-15</v>
+      </c>
       <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
@@ -913,7 +950,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>27</v>
       </c>
@@ -921,10 +958,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="17">
+      <c r="D15" s="6">
         <v>1020000000</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3455999999999998E-15</v>
+      </c>
       <c r="F15" s="4" t="s">
         <v>19</v>
       </c>
@@ -935,7 +975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>29</v>
       </c>
@@ -943,10 +983,13 @@
         <v>18</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="17">
+      <c r="D16" s="6">
         <v>600000000</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="6">
+        <f t="shared" si="0"/>
+        <v>1.968E-15</v>
+      </c>
       <c r="F16" s="4" t="s">
         <v>30</v>
       </c>
@@ -955,7 +998,7 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>31</v>
       </c>
@@ -963,10 +1006,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="17">
+      <c r="D17" s="6">
         <v>609000000</v>
       </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9975199999999998E-15</v>
+      </c>
       <c r="F17" s="4" t="s">
         <v>19</v>
       </c>
@@ -977,7 +1023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>32</v>
       </c>
@@ -985,10 +1031,13 @@
         <v>18</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="17">
+      <c r="D18" s="6">
         <v>588000000</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9286400000000001E-15</v>
+      </c>
       <c r="F18" s="4" t="s">
         <v>30</v>
       </c>
@@ -997,7 +1046,7 @@
       </c>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>33</v>
       </c>
@@ -1005,10 +1054,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="17">
+      <c r="D19" s="6">
         <v>203000000</v>
       </c>
-      <c r="E19" s="10"/>
+      <c r="E19" s="6">
+        <f t="shared" si="0"/>
+        <v>6.6583999999999999E-16</v>
+      </c>
       <c r="F19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1019,7 +1071,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>1316.5419999999999</v>
       </c>
@@ -1027,10 +1079,13 @@
         <v>18</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="17">
+      <c r="D20" s="6">
         <v>552000000</v>
       </c>
-      <c r="E20" s="10"/>
+      <c r="E20" s="6">
+        <f t="shared" si="0"/>
+        <v>1.81056E-15</v>
+      </c>
       <c r="F20" s="4" t="s">
         <v>13</v>
       </c>
@@ -1039,7 +1094,7 @@
       </c>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>34</v>
       </c>
@@ -1047,10 +1102,13 @@
         <v>18</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" s="17">
+      <c r="D21" s="6">
         <v>105000000</v>
       </c>
-      <c r="E21" s="10"/>
+      <c r="E21" s="6">
+        <f t="shared" si="0"/>
+        <v>3.4439999999999999E-16</v>
+      </c>
       <c r="F21" s="4" t="s">
         <v>13</v>
       </c>
@@ -1059,15 +1117,19 @@
       </c>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>1323.5150000000001</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="6">
         <v>302000000</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="0"/>
+        <v>9.9056000000000007E-16</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>13</v>
@@ -1079,15 +1141,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>1323.5219999999999</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="6">
         <v>102000000</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3456000000000001E-16</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>13</v>
@@ -1096,7 +1162,7 @@
         <v>34000000</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>36</v>
       </c>
@@ -1104,10 +1170,13 @@
         <v>9</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="17">
+      <c r="D24" s="6">
         <v>1680000000</v>
       </c>
-      <c r="E24" s="10"/>
+      <c r="E24" s="6">
+        <f t="shared" si="0"/>
+        <v>5.5103999999999998E-15</v>
+      </c>
       <c r="F24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1118,15 +1187,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="6">
         <v>44000000</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4432E-16</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>7</v>
@@ -1135,15 +1208,19 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="6">
         <v>1630000</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3463999999999995E-18</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>7</v>
@@ -1152,15 +1229,19 @@
         <v>542000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="6">
         <v>1250000</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0999999999999998E-18</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>7</v>
@@ -1169,15 +1250,19 @@
         <v>1250000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>1388.4349999999999</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="6">
         <v>2770000</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="0"/>
+        <v>9.0856000000000004E-18</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>7</v>
@@ -1186,15 +1271,19 @@
         <v>554000</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>1389.693</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="6">
         <v>1400000</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="0"/>
+        <v>4.5919999999999999E-18</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>41</v>
@@ -1203,15 +1292,19 @@
         <v>230000</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>1392.588</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="6">
         <v>1550000</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="0"/>
+        <v>5.0840000000000001E-18</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>7</v>
@@ -1223,15 +1316,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <v>1396.1120000000001</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="6">
         <v>2880000</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="0"/>
+        <v>9.4463999999999993E-18</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>7</v>
@@ -1241,15 +1338,19 @@
       </c>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>1401.5139999999999</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="6">
         <v>4880</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6006399999999999E-20</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>7</v>
@@ -1261,15 +1362,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <v>1409.337</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="6">
         <v>130000000</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="0"/>
+        <v>4.2639999999999999E-16</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>7</v>
@@ -1278,35 +1383,35 @@
         <v>43500000</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="16">
-        <v>1425.2190000000001</v>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="17">
-        <v>31500000</v>
-      </c>
-      <c r="E34" s="10"/>
+      <c r="D34" s="6">
+        <v>2650000000</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="0"/>
+        <v>8.692E-15</v>
+      </c>
       <c r="F34" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G34" s="13">
-        <v>10500000</v>
-      </c>
-      <c r="H34" s="10"/>
+        <v>379000000</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="4"/>
       <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="9"/>
-      <c r="B36" s="4"/>
-      <c r="F36" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed spaces from .csv file
</commit_message>
<xml_diff>
--- a/data/bright_lines.xlsx
+++ b/data/bright_lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojoa\GitHub\io_brightness\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0853BF40-CD6A-4988-B1EB-218556258607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E713762-7A95-4DB4-B487-7082637E7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16230" yWindow="3700" windowWidth="7500" windowHeight="6000" xr2:uid="{DFAE8F92-55DC-47F1-9DEE-F1EEFF5E956D}"/>
+    <workbookView xWindow="12820" yWindow="6000" windowWidth="12290" windowHeight="9380" xr2:uid="{DFAE8F92-55DC-47F1-9DEE-F1EEFF5E956D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Brightness</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blended? </t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">S IV contributes negligibly </t>
+  </si>
+  <si>
+    <t>Width</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,22 +634,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -657,9 +657,11 @@
         <v>1152.1510000000001</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0.25</v>
+      </c>
       <c r="D2" s="6">
         <v>2640000000</v>
       </c>
@@ -668,13 +670,13 @@
         <v>8.6592E-15</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="6">
         <v>528000000</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -682,9 +684,11 @@
         <v>1188.7739999999999</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0.26</v>
+      </c>
       <c r="D3" s="6">
         <v>1400000000</v>
       </c>
@@ -693,7 +697,7 @@
         <v>4.5919999999999997E-15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="11">
         <v>233000000</v>
@@ -705,9 +709,11 @@
         <v>1190.2059999999999</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.4</v>
+      </c>
       <c r="D4" s="6">
         <v>122000000</v>
       </c>
@@ -716,7 +722,7 @@
         <v>4.0015999999999998E-16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="11">
         <v>40500000</v>
@@ -728,9 +734,11 @@
         <v>1194.0609999999999</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.4</v>
+      </c>
       <c r="D5" s="6">
         <v>269000000</v>
       </c>
@@ -739,7 +747,7 @@
         <v>8.8232000000000001E-16</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="11">
         <v>53800000</v>
@@ -748,12 +756,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
+      </c>
       <c r="D6" s="6">
         <v>463000000</v>
       </c>
@@ -762,7 +772,7 @@
         <v>1.51864E-15</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="11">
         <v>66200000</v>
@@ -771,10 +781,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>0.31</v>
       </c>
       <c r="D7" s="6">
         <v>236000000</v>
@@ -784,7 +797,7 @@
         <v>7.7407999999999995E-16</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="13">
         <v>59100000</v>
@@ -795,7 +808,10 @@
         <v>1204.335</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>0.31</v>
       </c>
       <c r="D8" s="6">
         <v>347000000</v>
@@ -805,7 +821,7 @@
         <v>1.1381599999999999E-15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="13">
         <v>57900000</v>
@@ -816,7 +832,10 @@
         <v>1250.578</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>0.31</v>
       </c>
       <c r="D9" s="6">
         <v>347000000</v>
@@ -826,21 +845,24 @@
         <v>1.1381599999999999E-15</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="13">
         <v>51300000</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0.23</v>
       </c>
       <c r="D10" s="6">
         <v>7980000</v>
@@ -850,7 +872,7 @@
         <v>2.6174399999999998E-17</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" s="13">
         <v>2660000</v>
@@ -859,10 +881,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>0.31</v>
       </c>
       <c r="D11" s="6">
         <v>205000000</v>
@@ -872,13 +897,13 @@
         <v>6.7239999999999994E-16</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="13">
         <v>51200000</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -886,7 +911,10 @@
         <v>1259.518</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>0.31</v>
       </c>
       <c r="D12" s="6">
         <v>306000000</v>
@@ -896,21 +924,24 @@
         <v>1.00368E-15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="13">
         <v>51000000</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>0.23</v>
       </c>
       <c r="D13" s="6">
         <v>178000000</v>
@@ -920,7 +951,7 @@
         <v>5.8383999999999994E-16</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" s="13">
         <v>25400000</v>
@@ -929,12 +960,14 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>0.23</v>
+      </c>
       <c r="D14" s="6">
         <v>1730000000</v>
       </c>
@@ -943,7 +976,7 @@
         <v>5.6744000000000001E-15</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" s="6">
         <v>346000000</v>
@@ -952,12 +985,14 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>0.25</v>
+      </c>
       <c r="D15" s="6">
         <v>1020000000</v>
       </c>
@@ -966,23 +1001,25 @@
         <v>3.3455999999999998E-15</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="13">
         <v>341000000</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>0.23</v>
+      </c>
       <c r="D16" s="6">
         <v>600000000</v>
       </c>
@@ -991,7 +1028,7 @@
         <v>1.968E-15</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="13">
         <v>120000000</v>
@@ -1000,12 +1037,14 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>0.25</v>
+      </c>
       <c r="D17" s="6">
         <v>609000000</v>
       </c>
@@ -1014,23 +1053,25 @@
         <v>1.9975199999999998E-15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" s="13">
         <v>203000000</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.23</v>
+      </c>
       <c r="D18" s="6">
         <v>588000000</v>
       </c>
@@ -1039,7 +1080,7 @@
         <v>1.9286400000000001E-15</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="13">
         <v>196000000</v>
@@ -1048,12 +1089,14 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>0.25</v>
+      </c>
       <c r="D19" s="6">
         <v>203000000</v>
       </c>
@@ -1062,13 +1105,13 @@
         <v>6.6583999999999999E-16</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" s="13">
         <v>67600000</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1076,9 +1119,11 @@
         <v>1316.5419999999999</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>0.23</v>
+      </c>
       <c r="D20" s="6">
         <v>552000000</v>
       </c>
@@ -1087,7 +1132,7 @@
         <v>1.81056E-15</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" s="13">
         <v>78900000</v>
@@ -1096,12 +1141,14 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0.23</v>
+      </c>
       <c r="D21" s="6">
         <v>105000000</v>
       </c>
@@ -1110,7 +1157,7 @@
         <v>3.4439999999999999E-16</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21" s="13">
         <v>21000000</v>
@@ -1122,7 +1169,10 @@
         <v>1323.5150000000001</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>0.23</v>
       </c>
       <c r="D22" s="6">
         <v>302000000</v>
@@ -1132,13 +1182,13 @@
         <v>9.9056000000000007E-16</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="13">
         <v>60400000</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1146,7 +1196,10 @@
         <v>1323.5219999999999</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>0.23</v>
       </c>
       <c r="D23" s="6">
         <v>102000000</v>
@@ -1156,7 +1209,7 @@
         <v>3.3456000000000001E-16</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" s="13">
         <v>34000000</v>
@@ -1164,12 +1217,14 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>0.26</v>
+      </c>
       <c r="D24" s="6">
         <v>1680000000</v>
       </c>
@@ -1178,21 +1233,24 @@
         <v>5.5103999999999998E-15</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G24" s="13">
         <v>419000000</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>0.26</v>
       </c>
       <c r="D25" s="6">
         <v>44000000</v>
@@ -1202,7 +1260,7 @@
         <v>1.4432E-16</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25" s="13">
         <v>11000000</v>
@@ -1210,10 +1268,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>0.23</v>
       </c>
       <c r="D26" s="6">
         <v>1630000</v>
@@ -1223,7 +1284,7 @@
         <v>5.3463999999999995E-18</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G26" s="13">
         <v>542000</v>
@@ -1231,10 +1292,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.23</v>
       </c>
       <c r="D27" s="6">
         <v>1250000</v>
@@ -1244,7 +1308,7 @@
         <v>4.0999999999999998E-18</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G27" s="13">
         <v>1250000</v>
@@ -1255,7 +1319,10 @@
         <v>1388.4349999999999</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>0.23</v>
       </c>
       <c r="D28" s="6">
         <v>2770000</v>
@@ -1265,7 +1332,7 @@
         <v>9.0856000000000004E-18</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G28" s="13">
         <v>554000</v>
@@ -1276,7 +1343,10 @@
         <v>1389.693</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>0.26</v>
       </c>
       <c r="D29" s="6">
         <v>1400000</v>
@@ -1286,7 +1356,7 @@
         <v>4.5919999999999999E-18</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G29" s="13">
         <v>230000</v>
@@ -1297,7 +1367,10 @@
         <v>1392.588</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>0.23</v>
       </c>
       <c r="D30" s="6">
         <v>1550000</v>
@@ -1307,13 +1380,13 @@
         <v>5.0840000000000001E-18</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G30" s="13">
         <v>516000</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1321,7 +1394,10 @@
         <v>1396.1120000000001</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>0.23</v>
       </c>
       <c r="D31" s="6">
         <v>2880000</v>
@@ -1331,7 +1407,7 @@
         <v>9.4463999999999993E-18</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G31" s="13">
         <v>575000</v>
@@ -1343,7 +1419,10 @@
         <v>1401.5139999999999</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>0.23</v>
       </c>
       <c r="D32" s="6">
         <v>4880</v>
@@ -1353,13 +1432,13 @@
         <v>1.6006399999999999E-20</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G32" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1367,7 +1446,10 @@
         <v>1409.337</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <v>0.23</v>
       </c>
       <c r="D33" s="6">
         <v>130000000</v>
@@ -1377,7 +1459,7 @@
         <v>4.2639999999999999E-16</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G33" s="13">
         <v>43500000</v>
@@ -1385,12 +1467,14 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>0.23</v>
+      </c>
       <c r="D34" s="6">
         <v>2650000000</v>
       </c>
@@ -1399,13 +1483,13 @@
         <v>8.692E-15</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G34" s="13">
         <v>379000000</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>